<commit_message>
Mass commit, updated boards and project, depricated all old files
</commit_message>
<xml_diff>
--- a/Clock_PartsList.xlsx
+++ b/Clock_PartsList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdiro\Desktop\NixieClockRev2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC7E459-7343-4450-8246-04584BE25707}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD790D0B-47CA-47DA-9653-34E5361F6880}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6045" yWindow="5505" windowWidth="28800" windowHeight="12690" xr2:uid="{9419127E-C365-4B28-B0E7-0B6ADC239E75}"/>
+    <workbookView xWindow="4500" yWindow="4500" windowWidth="26460" windowHeight="13860" xr2:uid="{9419127E-C365-4B28-B0E7-0B6ADC239E75}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Digi-Key Part Number</t>
   </si>
@@ -45,26 +45,32 @@
     <t>RNCP0805FTD20K0CT-ND</t>
   </si>
   <si>
-    <t>160-1827-1-ND</t>
-  </si>
-  <si>
-    <t>D1-12</t>
-  </si>
-  <si>
-    <t>R1-12</t>
-  </si>
-  <si>
-    <t>R13-18</t>
-  </si>
-  <si>
-    <t>RR08P100DCT-ND</t>
+    <t>732-5309-ND</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>R1-6</t>
+  </si>
+  <si>
+    <t>R7-12</t>
+  </si>
+  <si>
+    <t>RR08P15.0KDCT-ND</t>
+  </si>
+  <si>
+    <t>1568-1800-ND</t>
+  </si>
+  <si>
+    <t>D1-6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,6 +105,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -127,7 +140,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -135,6 +148,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -453,7 +467,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,13 +489,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -489,10 +503,10 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
         <v>6</v>
-      </c>
-      <c r="C3">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -500,14 +514,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>

</xml_diff>